<commit_message>
new analysis and adjustment
script now runs in vscode
</commit_message>
<xml_diff>
--- a/data_tables/LoRRca_deformability.xlsx
+++ b/data_tables/LoRRca_deformability.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miri\Desktop\R\R-graphs\data_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miri\Documents\GitHub\R-graphs\data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53025E5B-8FB6-4FE8-AB35-289C7E7CD85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58641885-BB6D-4607-A98A-D3AF7A671EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20220" yWindow="960" windowWidth="21600" windowHeight="11175" xr2:uid="{CD73AF46-5553-49B2-86D2-713142B38856}"/>
+    <workbookView xWindow="6585" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{CD73AF46-5553-49B2-86D2-713142B38856}"/>
   </bookViews>
   <sheets>
     <sheet name="blank" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="6">
   <si>
     <t>EI</t>
   </si>
@@ -63,7 +52,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,7 +92,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1444E5-57B1-4D19-9269-260DDF9AE23C}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A101" activeCellId="3" sqref="A74 A83 A92 A101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0.106333333333333</v>
       </c>
@@ -465,7 +454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>0.17733333333333334</v>
       </c>
@@ -476,7 +465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>0.27299999999999996</v>
       </c>
@@ -487,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>0.34966666666666663</v>
       </c>
@@ -498,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>0.42333333333333334</v>
       </c>
@@ -509,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>0.49033333333333334</v>
       </c>
@@ -520,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>0.53800000000000003</v>
       </c>
@@ -531,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>0.57566666666666666</v>
       </c>
@@ -542,7 +531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>0.60699999999999998</v>
       </c>
@@ -553,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>0.111</v>
       </c>
@@ -564,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>0.17600000000000002</v>
       </c>
@@ -575,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>0.27300000000000002</v>
       </c>
@@ -586,7 +575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>0.36199999999999993</v>
       </c>
@@ -597,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>0.4286666666666667</v>
       </c>
@@ -608,7 +597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>0.49199999999999999</v>
       </c>
@@ -619,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>0.53533333333333333</v>
       </c>
@@ -630,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>0.57166666666666666</v>
       </c>
@@ -641,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>0.60433333333333328</v>
       </c>
@@ -652,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>0.10333333333333333</v>
       </c>
@@ -663,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>0.17300000000000001</v>
       </c>
@@ -674,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>0.27266666666666667</v>
       </c>
@@ -685,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>0.35200000000000004</v>
       </c>
@@ -696,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>0.42433333333333328</v>
       </c>
@@ -707,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>0.48933333333333334</v>
       </c>
@@ -718,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>0.53566666666666674</v>
       </c>
@@ -729,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>0.57233333333333325</v>
       </c>
@@ -740,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>0.60399999999999998</v>
       </c>
@@ -751,108 +740,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
-        <v>8.6333333333333331E-2</v>
+        <v>9.6000000000000016E-2</v>
       </c>
       <c r="B29">
         <v>0.3</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
-        <v>0.15533333333333332</v>
+        <v>0.15866666666666665</v>
       </c>
       <c r="B30">
         <v>0.53</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
-        <v>0.25666666666666665</v>
+        <v>0.27133333333333332</v>
       </c>
       <c r="B31">
         <v>0.95</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
-        <v>0.33966666666666662</v>
+        <v>0.35400000000000004</v>
       </c>
       <c r="B32">
         <v>1.69</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
-        <v>0.41566666666666663</v>
+        <v>0.43033333333333329</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
-        <v>0.48599999999999999</v>
+        <v>0.49233333333333329</v>
       </c>
       <c r="B34">
         <v>5.33</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
-        <v>0.53733333333333333</v>
+        <v>0.53833333333333333</v>
       </c>
       <c r="B35">
         <v>9.49</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
-        <v>0.56366666666666665</v>
+        <v>0.57466666666666666</v>
       </c>
       <c r="B36">
         <v>16.87</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
-        <v>0.60733333333333339</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="B37">
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
-        <v>0.10566666666666667</v>
+        <v>8.6333333333333331E-2</v>
       </c>
       <c r="B38">
         <v>0.3</v>
@@ -861,9 +850,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
-        <v>0.15833333333333333</v>
+        <v>0.15533333333333332</v>
       </c>
       <c r="B39">
         <v>0.53</v>
@@ -872,9 +861,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
-        <v>0.25933333333333336</v>
+        <v>0.25666666666666665</v>
       </c>
       <c r="B40">
         <v>0.95</v>
@@ -883,9 +872,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
-        <v>0.35033333333333333</v>
+        <v>0.33966666666666662</v>
       </c>
       <c r="B41">
         <v>1.69</v>
@@ -894,9 +883,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
-        <v>0.42</v>
+        <v>0.41566666666666663</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -905,9 +894,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
-        <v>0.48533333333333334</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="B43">
         <v>5.33</v>
@@ -916,9 +905,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
-        <v>0.53233333333333344</v>
+        <v>0.53733333333333333</v>
       </c>
       <c r="B44">
         <v>9.49</v>
@@ -927,9 +916,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.56366666666666665</v>
       </c>
       <c r="B45">
         <v>16.87</v>
@@ -938,9 +927,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
-        <v>0.60233333333333328</v>
+        <v>0.60733333333333339</v>
       </c>
       <c r="B46">
         <v>30</v>
@@ -949,9 +938,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
-        <v>9.2666666666666675E-2</v>
+        <v>0.10566666666666667</v>
       </c>
       <c r="B47">
         <v>0.3</v>
@@ -960,9 +949,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
-        <v>0.16</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="B48">
         <v>0.53</v>
@@ -971,7 +960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>0.25933333333333336</v>
       </c>
@@ -982,9 +971,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
-        <v>0.35299999999999998</v>
+        <v>0.35033333333333333</v>
       </c>
       <c r="B50">
         <v>1.69</v>
@@ -993,9 +982,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
-        <v>0.39733333333333332</v>
+        <v>0.42</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -1004,9 +993,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
-        <v>0.49033333333333334</v>
+        <v>0.48533333333333334</v>
       </c>
       <c r="B52">
         <v>5.33</v>
@@ -1015,9 +1004,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
-        <v>0.53700000000000003</v>
+        <v>0.53233333333333344</v>
       </c>
       <c r="B53">
         <v>9.49</v>
@@ -1026,9 +1015,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
-        <v>0.57499999999999984</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="B54">
         <v>16.87</v>
@@ -1037,9 +1026,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
-        <v>0.60566666666666669</v>
+        <v>0.60233333333333328</v>
       </c>
       <c r="B55">
         <v>30</v>
@@ -1048,207 +1037,207 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
-        <v>8.6333333333333331E-2</v>
+        <v>9.2666666666666675E-2</v>
       </c>
       <c r="B56">
         <v>0.3</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
-        <v>0.14566666666666669</v>
+        <v>0.16</v>
       </c>
       <c r="B57">
         <v>0.53</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
-        <v>0.24766666666666667</v>
+        <v>0.25933333333333336</v>
       </c>
       <c r="B58">
         <v>0.95</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
-        <v>0.33733333333333332</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="B59">
         <v>1.69</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
-        <v>0.41166666666666663</v>
+        <v>0.39733333333333332</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
-        <v>0.48199999999999998</v>
+        <v>0.49033333333333334</v>
       </c>
       <c r="B61">
         <v>5.33</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
-        <v>0.53166666666666673</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="B62">
         <v>9.49</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.57499999999999984</v>
       </c>
       <c r="B63">
         <v>16.87</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
-        <v>0.60333333333333339</v>
+        <v>0.60566666666666669</v>
       </c>
       <c r="B64">
         <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
-        <v>8.7666666666666671E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="B65">
         <v>0.3</v>
       </c>
       <c r="C65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
-        <v>0.156</v>
+        <v>0.14833333333333332</v>
       </c>
       <c r="B66">
         <v>0.53</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
-        <v>0.25566666666666665</v>
+        <v>0.25033333333333335</v>
       </c>
       <c r="B67">
         <v>0.95</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
-        <v>0.34666666666666668</v>
+        <v>0.34199999999999992</v>
       </c>
       <c r="B68">
         <v>1.69</v>
       </c>
       <c r="C68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
-        <v>0.41733333333333333</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="B69">
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
-        <v>0.48399999999999999</v>
+        <v>0.49433333333333335</v>
       </c>
       <c r="B70">
         <v>5.33</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
-        <v>0.53300000000000003</v>
+        <v>0.54633333333333345</v>
       </c>
       <c r="B71">
         <v>9.49</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
-        <v>0.56966666666666665</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="B72">
         <v>16.87</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
-        <v>0.60166666666666668</v>
+        <v>0.61366666666666669</v>
       </c>
       <c r="B73">
         <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
-        <v>9.3333333333333338E-2</v>
+        <v>8.6333333333333331E-2</v>
       </c>
       <c r="B74">
         <v>0.3</v>
@@ -1257,9 +1246,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
-        <v>0.153</v>
+        <v>0.14566666666666669</v>
       </c>
       <c r="B75">
         <v>0.53</v>
@@ -1268,9 +1257,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
-        <v>0.254</v>
+        <v>0.24766666666666667</v>
       </c>
       <c r="B76">
         <v>0.95</v>
@@ -1279,9 +1268,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
-        <v>0.34466666666666662</v>
+        <v>0.33733333333333332</v>
       </c>
       <c r="B77">
         <v>1.69</v>
@@ -1290,9 +1279,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
-        <v>0.41933333333333334</v>
+        <v>0.41166666666666663</v>
       </c>
       <c r="B78">
         <v>3</v>
@@ -1301,9 +1290,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
-        <v>0.48599999999999999</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="B79">
         <v>5.33</v>
@@ -1312,9 +1301,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
-        <v>0.53466666666666673</v>
+        <v>0.53166666666666673</v>
       </c>
       <c r="B80">
         <v>9.49</v>
@@ -1323,9 +1312,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
-        <v>0.57299999999999995</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="B81">
         <v>16.87</v>
@@ -1334,14 +1323,311 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
-        <v>0.60466666666666657</v>
+        <v>0.60333333333333339</v>
       </c>
       <c r="B82">
         <v>30</v>
       </c>
       <c r="C82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>8.7666666666666671E-2</v>
+      </c>
+      <c r="B83">
+        <v>0.3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>0.156</v>
+      </c>
+      <c r="B84">
+        <v>0.53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>0.25566666666666665</v>
+      </c>
+      <c r="B85">
+        <v>0.95</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>0.34666666666666668</v>
+      </c>
+      <c r="B86">
+        <v>1.69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>0.41733333333333333</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="B88">
+        <v>5.33</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="B89">
+        <v>9.49</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>0.56966666666666665</v>
+      </c>
+      <c r="B90">
+        <v>16.87</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>0.60166666666666668</v>
+      </c>
+      <c r="B91">
+        <v>30</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>9.3333333333333338E-2</v>
+      </c>
+      <c r="B92">
+        <v>0.3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
+        <v>0.153</v>
+      </c>
+      <c r="B93">
+        <v>0.53</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
+        <v>0.254</v>
+      </c>
+      <c r="B94">
+        <v>0.95</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
+        <v>0.34466666666666662</v>
+      </c>
+      <c r="B95">
+        <v>1.69</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
+        <v>0.41933333333333334</v>
+      </c>
+      <c r="B96">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="B97">
+        <v>5.33</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1">
+        <v>0.53466666666666673</v>
+      </c>
+      <c r="B98">
+        <v>9.49</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="B99">
+        <v>16.87</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1">
+        <v>0.60466666666666657</v>
+      </c>
+      <c r="B100">
+        <v>30</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1">
+        <v>6.433333333333334E-2</v>
+      </c>
+      <c r="B101">
+        <v>0.3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1">
+        <v>0.12533333333333332</v>
+      </c>
+      <c r="B102">
+        <v>0.53</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1">
+        <v>0.23033333333333336</v>
+      </c>
+      <c r="B103">
+        <v>0.95</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1">
+        <v>0.3136666666666667</v>
+      </c>
+      <c r="B104">
+        <v>1.69</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1">
+        <v>0.40166666666666667</v>
+      </c>
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="B106">
+        <v>5.33</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="B107">
+        <v>9.49</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1">
+        <v>0.57566666666666666</v>
+      </c>
+      <c r="B108">
+        <v>16.87</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1">
+        <v>0.60866666666666669</v>
+      </c>
+      <c r="B109">
+        <v>30</v>
+      </c>
+      <c r="C109" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>